<commit_message>
Add canvas, transition. machine learning seconde commit
</commit_message>
<xml_diff>
--- a/FinalWebApp/FinalWebApp/TestData.xlsx
+++ b/FinalWebApp/FinalWebApp/TestData.xlsx
@@ -364,8 +364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A9" sqref="A1:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,19 +398,19 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -421,16 +421,16 @@
         <v>21</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -447,7 +447,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -516,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -539,7 +539,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -591,7 +591,7 @@
         <v>3</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -614,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>9</v>
@@ -651,19 +651,19 @@
         <v>32</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -674,19 +674,19 @@
         <v>33</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>11</v>
@@ -697,13 +697,13 @@
         <v>34</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>4</v>
@@ -798,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>4</v>
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -855,5 +855,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>